<commit_message>
three leaves from three trees release
+ fixes for a smooth bookdown production chain
+ svmono class
+ faulty formulas fixed
+ removed colons from chunk names
+ fixed all bookdown yaml configs
</commit_message>
<xml_diff>
--- a/Illustrations/GLM_distributions.xlsx
+++ b/Illustrations/GLM_distributions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schme\Google Drive\Aktenkoffer\Publications\New_Stats\figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmettowm\Google Drive\Aktenkoffer\Publications\New_Stats\Illustrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="0" windowWidth="14400" windowHeight="20052" activeTab="1"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="14400" windowHeight="20055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -84,22 +84,22 @@
     <t>gamma</t>
   </si>
   <si>
-    <t>$$\alpha \gt 0\\ \beta \gt 0$$</t>
-  </si>
-  <si>
     <t>limiting case</t>
   </si>
   <si>
-    <t>$$\alpha, \beta \rightarrow \infty$$</t>
-  </si>
-  <si>
     <t>rate, shape</t>
+  </si>
+  <si>
+    <t>$\alpha, \beta \rightarrow \infty$</t>
+  </si>
+  <si>
+    <t>$\alpha &gt; 0, \beta &gt; 0$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,13 +417,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -434,7 +434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -442,7 +442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -453,7 +453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -474,18 +474,18 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -496,10 +496,10 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -507,13 +507,13 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -521,7 +521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -529,7 +529,7 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>